<commit_message>
Uploaded IEP data for years ending in 2010-2015 and combined them into one iep_comb dataset.
</commit_message>
<xml_diff>
--- a/demo_data/Thesis_demographic_data/2014_schooldemo.xlsx
+++ b/demo_data/Thesis_demographic_data/2014_schooldemo.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amytan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amytan/Desktop/Gov 1005_Data/chicago_isat/demo_data/Thesis_demographic_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="3360" yWindow="10700" windowWidth="27760" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Educational Units" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -2289,10 +2289,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2575,7 +2575,7 @@
   <dimension ref="A1:Y673"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
@@ -2609,42 +2609,42 @@
   <sheetData>
     <row r="1" spans="1:25" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1"/>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="20" t="s">
         <v>702</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="20" t="s">
+      <c r="H1" s="20"/>
+      <c r="I1" s="21" t="s">
         <v>701</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20" t="s">
+      <c r="J1" s="21"/>
+      <c r="K1" s="21" t="s">
         <v>700</v>
       </c>
-      <c r="L1" s="20"/>
-      <c r="M1" s="21" t="s">
+      <c r="L1" s="21"/>
+      <c r="M1" s="20" t="s">
         <v>699</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="20" t="s">
+      <c r="N1" s="20"/>
+      <c r="O1" s="21" t="s">
         <v>698</v>
       </c>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="21" t="s">
+      <c r="P1" s="21"/>
+      <c r="Q1" s="20" t="s">
         <v>697</v>
       </c>
-      <c r="R1" s="21"/>
-      <c r="S1" s="20" t="s">
+      <c r="R1" s="20"/>
+      <c r="S1" s="21" t="s">
         <v>696</v>
       </c>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20" t="s">
+      <c r="T1" s="21"/>
+      <c r="U1" s="21" t="s">
         <v>695</v>
       </c>
-      <c r="V1" s="20"/>
+      <c r="V1" s="21"/>
       <c r="W1" s="1"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="1"/>

</xml_diff>